<commit_message>
Update Realisasi 13 Feb 2023 (3,91%)
</commit_message>
<xml_diff>
--- a/Database/MONSAKTI/MONITORING BELANJA SPM LS.xlsx
+++ b/Database/MONSAKTI/MONITORING BELANJA SPM LS.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="220">
   <si>
     <t>MONITORING BELANJA SPM LS</t>
   </si>
@@ -104,30 +104,30 @@
     <t>Pembayaran belanja pegawai(pembayaran gaji susulan pegawai Sekretariat BRSDMKP bulan Januari 2023 untuk 1 pegawai/1 Jiwa)</t>
   </si>
   <si>
+    <t>'00006T</t>
+  </si>
+  <si>
+    <t>16-JAN-23</t>
+  </si>
+  <si>
+    <t>'00006A</t>
+  </si>
+  <si>
+    <t>17-JAN-23</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Pegawai (Pembayaran Gaji Induk Pegawai Set.BRSDM Bulan Februari Tahun 2023 untuk 77 pegawai 204 jiwa)</t>
+  </si>
+  <si>
     <t>'00007T</t>
   </si>
   <si>
-    <t>16-JAN-23</t>
-  </si>
-  <si>
     <t>'00007A</t>
   </si>
   <si>
-    <t>17-JAN-23</t>
-  </si>
-  <si>
     <t>Pembayaran Belanja Pegawai (Pembayaran Gaji Induk Pegawai Pusdik KP Bulan Februari Tahun 2023 Untuk 44 pegawai 120 jiwa)</t>
   </si>
   <si>
-    <t>'00006T</t>
-  </si>
-  <si>
-    <t>'00006A</t>
-  </si>
-  <si>
-    <t>Pembayaran Belanja Pegawai (Pembayaran Gaji Induk Pegawai Set.BRSDM Bulan Februari Tahun 2023 untuk 77 pegawai 204 jiwa)</t>
-  </si>
-  <si>
     <t>'00008T</t>
   </si>
   <si>
@@ -137,12 +137,24 @@
     <t>Pembayaran Belanja Pegawai (Pembayaran Gaji Induk Puslatluh KP Bulan Februari 2023 Untuk 39 pegawai 110 jiwa)</t>
   </si>
   <si>
+    <t>'00011T</t>
+  </si>
+  <si>
+    <t>20-JAN-23</t>
+  </si>
+  <si>
+    <t>'00011A</t>
+  </si>
+  <si>
+    <t>25-JAN-23</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Berupa Honor PPNPN Pusat Pendidikan KP Bulan Januari Tahun 2023 untuk 13 Pegawai sesuai Surat Keputusan Nomor KEP 2/KPA/BRSDM/2023 tgl 2 Januari 2023</t>
+  </si>
+  <si>
     <t>'00010T</t>
   </si>
   <si>
-    <t>20-JAN-23</t>
-  </si>
-  <si>
     <t>'00010A</t>
   </si>
   <si>
@@ -161,16 +173,94 @@
     <t>Pembayaran Belanja Barang Sesuai Kwitansi Nomor:34294364,34293709,34294166 Tanggal 11 Januari 2023</t>
   </si>
   <si>
-    <t>'00011T</t>
-  </si>
-  <si>
-    <t>'00011A</t>
-  </si>
-  <si>
-    <t>25-JAN-23</t>
-  </si>
-  <si>
-    <t>Pembayaran Belanja Barang Berupa Honor PPNPN Pusat Pendidikan KP Bulan Januari Tahun 2023 untuk 13 Pegawai sesuai Surat Keputusan Nomor KEP 2/KPA/BRSDM/2023 tgl 2 Januari 2023</t>
+    <t>'00012T</t>
+  </si>
+  <si>
+    <t>'00012A</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Berupa Honor PPNPN Bulan Januari Tahun 2023 untuk 40 Pegawai Sesuai Surat Keputusan Nomor:KEP.1/KPA/BRSDM/I/2023 Tanggal 02 Januari 2023</t>
+  </si>
+  <si>
+    <t>'00013T</t>
+  </si>
+  <si>
+    <t>'00013A</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang sesuai surat keputusan No.KEP.3/KPA/BRSDM/I/2023.Tgl.02 Januari 2023,gaji PPNPN Bulan Januari Tahun 2023 untuk 16 Pegawai.</t>
+  </si>
+  <si>
+    <t>'00016T</t>
+  </si>
+  <si>
+    <t>'00016A</t>
+  </si>
+  <si>
+    <t>EBD</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.200/BRSDM.1/KP.440/I/2023 Tanggal 6 Januari 2023</t>
+  </si>
+  <si>
+    <t>'00021T</t>
+  </si>
+  <si>
+    <t>'00021A</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.370/BRSDM.1/KP.440/I/2023 Tanggal 16 Januari 2023</t>
+  </si>
+  <si>
+    <t>'00025T</t>
+  </si>
+  <si>
+    <t>'00025A</t>
+  </si>
+  <si>
+    <t>Pembayara Belanja Barang Sesuai Surat Tugas Nomor:B.200/BRSDM.1/KP.440/I/2023 Tanggal 6 Januari 2023</t>
+  </si>
+  <si>
+    <t>'00017T</t>
+  </si>
+  <si>
+    <t>'00017A</t>
+  </si>
+  <si>
+    <t>'00022T</t>
+  </si>
+  <si>
+    <t>'00022A</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.303,B.304/BRSDM.1/KP.440/I/2023 Tanggal 10 Januari 2023</t>
+  </si>
+  <si>
+    <t>'00018T</t>
+  </si>
+  <si>
+    <t>'00018A</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.141/BRSDM.1/KP.440/I/2023 Tanggal 4 Januari 2023</t>
+  </si>
+  <si>
+    <t>'00023T</t>
+  </si>
+  <si>
+    <t>'00023A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.143/BRSDM.1/KP.440/I/2023 Tanggal 4 Januari 2023 </t>
+  </si>
+  <si>
+    <t>'00019T</t>
+  </si>
+  <si>
+    <t>'00019A</t>
+  </si>
+  <si>
+    <t>EBC</t>
   </si>
   <si>
     <t>'00024T</t>
@@ -179,9 +269,6 @@
     <t>'00024A</t>
   </si>
   <si>
-    <t>EBD</t>
-  </si>
-  <si>
     <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.414/BRSDM.1/KP.440/I/2023 Tanggal 18 Januari 2023</t>
   </si>
   <si>
@@ -191,9 +278,6 @@
     <t>'00020A</t>
   </si>
   <si>
-    <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.200/BRSDM.1/KP.440/I/2023 Tanggal 6 Januari 2023</t>
-  </si>
-  <si>
     <t>'00015T</t>
   </si>
   <si>
@@ -203,90 +287,6 @@
     <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.201/BRSDM.1/KP.440/I/2023 Tanggal 6 Januari 2023</t>
   </si>
   <si>
-    <t>'00016T</t>
-  </si>
-  <si>
-    <t>'00016A</t>
-  </si>
-  <si>
-    <t>'00021T</t>
-  </si>
-  <si>
-    <t>'00021A</t>
-  </si>
-  <si>
-    <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.370/BRSDM.1/KP.440/I/2023 Tanggal 16 Januari 2023</t>
-  </si>
-  <si>
-    <t>'00012T</t>
-  </si>
-  <si>
-    <t>'00012A</t>
-  </si>
-  <si>
-    <t>Pembayaran Belanja Barang Berupa Honor PPNPN Bulan Januari Tahun 2023 untuk 40 Pegawai Sesuai Surat Keputusan Nomor:KEP.1/KPA/BRSDM/I/2023 Tanggal 02 Januari 2023</t>
-  </si>
-  <si>
-    <t>'00013T</t>
-  </si>
-  <si>
-    <t>'00013A</t>
-  </si>
-  <si>
-    <t>Pembayaran Belanja Barang sesuai surat keputusan No.KEP.3/KPA/BRSDM/I/2023.Tgl.02 Januari 2023,gaji PPNPN Bulan Januari Tahun 2023 untuk 16 Pegawai.</t>
-  </si>
-  <si>
-    <t>'00017T</t>
-  </si>
-  <si>
-    <t>'00017A</t>
-  </si>
-  <si>
-    <t>'00022T</t>
-  </si>
-  <si>
-    <t>'00022A</t>
-  </si>
-  <si>
-    <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.303,B.304/BRSDM.1/KP.440/I/2023 Tanggal 10 Januari 2023</t>
-  </si>
-  <si>
-    <t>'00018T</t>
-  </si>
-  <si>
-    <t>'00018A</t>
-  </si>
-  <si>
-    <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.141/BRSDM.1/KP.440/I/2023 Tanggal 4 Januari 2023</t>
-  </si>
-  <si>
-    <t>'00023T</t>
-  </si>
-  <si>
-    <t>'00023A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.143/BRSDM.1/KP.440/I/2023 Tanggal 4 Januari 2023 </t>
-  </si>
-  <si>
-    <t>'00019T</t>
-  </si>
-  <si>
-    <t>'00019A</t>
-  </si>
-  <si>
-    <t>EBC</t>
-  </si>
-  <si>
-    <t>'00025T</t>
-  </si>
-  <si>
-    <t>'00025A</t>
-  </si>
-  <si>
-    <t>Pembayara Belanja Barang Sesuai Surat Tugas Nomor:B.200/BRSDM.1/KP.440/I/2023 Tanggal 6 Januari 2023</t>
-  </si>
-  <si>
     <t>'00026T</t>
   </si>
   <si>
@@ -302,6 +302,15 @@
     <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.42/BRSDM.5/KP.440/I/2023 Tanggal 9 Januari 2023</t>
   </si>
   <si>
+    <t>'00028T</t>
+  </si>
+  <si>
+    <t>'00028A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pembayaran Belanja Barang Sesuai SPK No:SPK-141/PPK/BRSDM.1/I/20223 Tgl.11-1-2023,BAST No:BAST.181/PPK/BRSDM.1/I/2023 Tgl.13-1-2023,BAP No:BAP.182/PPK/BRSDM.1/I/2023 Tgl.13-1-2023 </t>
+  </si>
+  <si>
     <t>'00027T</t>
   </si>
   <si>
@@ -311,13 +320,55 @@
     <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.248,41/BRSDM/KP.440/I/2023 Tanggal 9 Januari 2023 dan No.B.41/BRSDM.5/KP.440/I/2023.Tgl.9 Januari 2023.</t>
   </si>
   <si>
-    <t>'00028T</t>
-  </si>
-  <si>
-    <t>'00028A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pembayaran Belanja Barang Sesuai SPK No:SPK-141/PPK/BRSDM.1/I/20223 Tgl.11-1-2023,BAST No:BAST.181/PPK/BRSDM.1/I/2023 Tgl.13-1-2023,BAP No:BAP.182/PPK/BRSDM.1/I/2023 Tgl.13-1-2023 </t>
+    <t>'00057T</t>
+  </si>
+  <si>
+    <t>'07-FEB-23</t>
+  </si>
+  <si>
+    <t>'00057A</t>
+  </si>
+  <si>
+    <t>Pembyaran Belanja Barang Sesuai Surat TUgas  Nomor:B.304/BRSDM.1/KP.440/I/2023 Tanggal 10 Januari 2023</t>
+  </si>
+  <si>
+    <t>'00058T</t>
+  </si>
+  <si>
+    <t>'00058A</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.309/BRSDM.1/KP.440/I/2023 Tanggal 10 Januari 2023</t>
+  </si>
+  <si>
+    <t>'00032T</t>
+  </si>
+  <si>
+    <t>31-JAN-23</t>
+  </si>
+  <si>
+    <t>'00032A</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Kwitansi Nomor:INV.001/RRM/I/2023 Tanggal 9 Januari 2023</t>
+  </si>
+  <si>
+    <t>'00029T</t>
+  </si>
+  <si>
+    <t>'00029A</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.303/BRSDM.1/KP.440/I/2023 Tanggal 10 Januari 2023</t>
+  </si>
+  <si>
+    <t>'00033T</t>
+  </si>
+  <si>
+    <t>'00033A</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.304/BRSDM.1/KP.440/I/2023 Tanggal 10 Januari 2023</t>
   </si>
   <si>
     <t>'00030T</t>
@@ -329,34 +380,13 @@
     <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.276/?BRSDM.1/TU.440/I/2023 Tanggal 10 Januari 2023</t>
   </si>
   <si>
-    <t>'00033T</t>
-  </si>
-  <si>
-    <t>31-JAN-23</t>
-  </si>
-  <si>
-    <t>'00033A</t>
-  </si>
-  <si>
-    <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.304/BRSDM.1/KP.440/I/2023 Tanggal 10 Januari 2023</t>
-  </si>
-  <si>
-    <t>'00032T</t>
-  </si>
-  <si>
-    <t>'00032A</t>
-  </si>
-  <si>
-    <t>Pembayaran Belanja Barang Sesuai Kwitansi Nomor:INV.001/RRM/I/2023 Tanggal 9 Januari 2023</t>
-  </si>
-  <si>
-    <t>'00029T</t>
-  </si>
-  <si>
-    <t>'00029A</t>
-  </si>
-  <si>
-    <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.303/BRSDM.1/KP.440/I/2023 Tanggal 10 Januari 2023</t>
+    <t>'00035T</t>
+  </si>
+  <si>
+    <t>'00035A</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.222/BRSDM.1/KP.440/I/2023 Tanggal 6 Januari 2023</t>
   </si>
   <si>
     <t>'00037T</t>
@@ -368,15 +398,6 @@
     <t>Pembayaran Belanja Barang Sesuai Kwitansi Nomor:006 Tanggal 9 Januari 2023</t>
   </si>
   <si>
-    <t>'00035T</t>
-  </si>
-  <si>
-    <t>'00035A</t>
-  </si>
-  <si>
-    <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.222/BRSDM.1/KP.440/I/2023 Tanggal 6 Januari 2023</t>
-  </si>
-  <si>
     <t>'00038T</t>
   </si>
   <si>
@@ -428,6 +449,15 @@
     <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor: B.513/BRSDM.1/KP.440/2023 tanggal 25 Januari 2023</t>
   </si>
   <si>
+    <t>'00044T</t>
+  </si>
+  <si>
+    <t>'00044A</t>
+  </si>
+  <si>
+    <t>Pembayaran belanja barang sesuai surat tugas nomor: B.456, B.483/BRSDM.1/KP.440/I/2023 tanggal 19 Januari 2023 dan 20 Januari 2023.</t>
+  </si>
+  <si>
     <t>'00045T</t>
   </si>
   <si>
@@ -437,21 +467,21 @@
     <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor: B.85/BRSDM.1/KP.440/2023 tanggal 16 Januari 2023</t>
   </si>
   <si>
-    <t>'00044T</t>
-  </si>
-  <si>
-    <t>'00044A</t>
-  </si>
-  <si>
-    <t>Pembayaran belanja barang sesuai surat tugas nomor: B.456, B.483/BRSDM.1/KP.440/I/2023 tanggal 19 Januari 2023 dan 20 Januari 2023.</t>
+    <t>'00049T</t>
+  </si>
+  <si>
+    <t>'03-FEB-23</t>
+  </si>
+  <si>
+    <t>'00049A</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Pegawai (Pembayaran Kekurangan Gaji Tunjangan Fungsional PNS Sekretariat BRSDM Untuk 4 Pegawai 16 Jiwa)</t>
   </si>
   <si>
     <t>'00047T</t>
   </si>
   <si>
-    <t>'03-FEB-23</t>
-  </si>
-  <si>
     <t>'00047A</t>
   </si>
   <si>
@@ -467,15 +497,6 @@
     <t>Pembayaran Belanja Pegawai (Pembayaran Kekurangan Gaji Tunjangan Fungsional PNS PUSDIK Bulan Januari 2023 Untuk 4 Pegawai 10 Jiwa)</t>
   </si>
   <si>
-    <t>'00049T</t>
-  </si>
-  <si>
-    <t>'00049A</t>
-  </si>
-  <si>
-    <t>Pembayaran Belanja Pegawai (Pembayaran Kekurangan Gaji Tunjangan Fungsional PNS Sekretariat BRSDM Untuk 4 Pegawai 16 Jiwa)</t>
-  </si>
-  <si>
     <t>'00050T</t>
   </si>
   <si>
@@ -485,88 +506,175 @@
     <t>Pembayaran Belanja Pegawai (Pembayaran Gaji Susulan PNS Pusdik Bulan Januari-Februari 2023 Untuk 1 Pegawai 1 Jiwa)</t>
   </si>
   <si>
-    <t>'00046T</t>
+    <t>'00053T</t>
   </si>
   <si>
     <t>'06-FEB-23</t>
   </si>
   <si>
+    <t>'00053A</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Pegawai (Pembayaran Tunjangan Kinerja PNS Puslatluh Bulan Januari 2023 Untuk 34 Pegawai)</t>
+  </si>
+  <si>
+    <t>'00054T</t>
+  </si>
+  <si>
+    <t>'00054A</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Kwitansi Nomor:016/JSA.1/KW.SET BRSDM/I/2023 Tanggal 24 Januari 2023</t>
+  </si>
+  <si>
+    <t>'00052T</t>
+  </si>
+  <si>
+    <t>'00052A</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Pegawai (Pembayaaran Tunjangan Kinerja PNS Set.BRSDM Bulan Januari 2023 Untuk 75 Pegawai)</t>
+  </si>
+  <si>
+    <t>'00051T</t>
+  </si>
+  <si>
+    <t>'00051A</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.342/BRSDM.1/KP.440/I/2023 Tanggal 16 Januari 2023</t>
+  </si>
+  <si>
+    <t>'00055T</t>
+  </si>
+  <si>
+    <t>'00055A</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Pegawai (Pembayaran Tunjangan Kinerja PNS Pusdik Bulan Januari 2023 untuk 42 Pegawai)</t>
+  </si>
+  <si>
+    <t>'00061T</t>
+  </si>
+  <si>
+    <t>'08-FEB-23</t>
+  </si>
+  <si>
+    <t>'00061A</t>
+  </si>
+  <si>
+    <t>EBB</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Modal Sesuai SPK No:341/PPK/BRSDM.1/I/2023 tgl.26-1-2023, BAST No:BAST.381/PPK/BRSDM.1/I/2023 tgl.30-1-2023, BAP NO:382/PPK/BRSDM.1/I/2023 tgl.30-1-2023 Pengadaan Infrastruktur/Sarpras Command Center</t>
+  </si>
+  <si>
+    <t>'00066T</t>
+  </si>
+  <si>
+    <t>'00066A</t>
+  </si>
+  <si>
+    <t>13-FEB-23</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang. Biaya hidup lanjutan tubel Prog S2 dan S3 IPB, UNDIP, AUP, UB dan UNS Periode Jan-Juni 2023 sesuai dengan SK Ka BRSDM KP No: 757/KPA/BRSDM/VIII/2021 Tgl 13-8-2021 dan 107/KEP-BRSDM/2020 Tgl 18-82020 an. Endang Puji Lestari, dkk</t>
+  </si>
+  <si>
+    <t>'00065T</t>
+  </si>
+  <si>
+    <t>'00065A</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang. Biaya hidup peserta lanjutan tubel Prog S2 dan S3 IPB, UNDIP, UNPAD, UB dan UNS Periode Jan-Juni 2023 sesuai dengan SK Ka BRSDM KP No: 520 Tahun 2022 Tgl 11 Agustus 2022 an. Fitriska Hapsyari Sutrisno, dkk</t>
+  </si>
+  <si>
+    <t>'00060T</t>
+  </si>
+  <si>
+    <t>'00060A</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Kwitansi Nomor:130001276 Tanggal 30 Januari 2023</t>
+  </si>
+  <si>
+    <t>'00062T</t>
+  </si>
+  <si>
+    <t>'00062A</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Modal Sesuai SPK No:343/PPK/BRSDM.1/I/2023 tgl.26-1-2023,BAST No:BAST.385/PPK/BRSDM.1/I/2023 tgl.30-1-2023,BAP No:386/PPK/BRSDM.1/2023 tgl.30-1-2023 Pengadaan media penayangan rapat konferensi</t>
+  </si>
+  <si>
+    <t>'00064T</t>
+  </si>
+  <si>
+    <t>'00064A</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang dalam rangka Pendampingan Kolaborasi Penyuluh dengan program Desa Perikanan Cerdas (SFV) Sesuai Surat Tugas Nomor:B.249/BRSDM.4/KP.440/I/2023 tanggal 24 Januari 2023</t>
+  </si>
+  <si>
+    <t>'00059T</t>
+  </si>
+  <si>
+    <t>'00059A</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Sesuai Kwitansi Nomor:1300031276 Tanggal 30 Januari 2023</t>
+  </si>
+  <si>
+    <t>'00067T</t>
+  </si>
+  <si>
+    <t>'09-FEB-23</t>
+  </si>
+  <si>
+    <t>'00067A</t>
+  </si>
+  <si>
     <t>Pembayaran Belanja Barang Berupa Honor PPNPN Bulan Januari Tahun 2023 untuk 2 Pegawai Sesuai Surat Keputusan Nomor:KEP.1/KPA/BRSDM/I/2023 Tanggal 02 Januari 2023</t>
   </si>
   <si>
-    <t>'00051T</t>
-  </si>
-  <si>
-    <t>'00051A</t>
-  </si>
-  <si>
-    <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.342/BRSDM.1/KP.440/I/2023 Tanggal 16 Januari 2023</t>
-  </si>
-  <si>
-    <t>'00053T</t>
-  </si>
-  <si>
-    <t>'00053A</t>
-  </si>
-  <si>
-    <t>Pembayaran Belanja Pegawai (Pembayaran Tunjangan Kinerja PNS Puslatluh Bulan Januari 2023 Untuk 34 Pegawai)</t>
-  </si>
-  <si>
-    <t>'00055T</t>
-  </si>
-  <si>
-    <t>'00055A</t>
-  </si>
-  <si>
-    <t>Pembayaran Belanja Pegawai (Pembayaran Tunjangan Kinerja PNS Pusdik Bulan Januari 2023 untuk 42 Pegawai)</t>
-  </si>
-  <si>
-    <t>'00054T</t>
-  </si>
-  <si>
-    <t>'00054A</t>
-  </si>
-  <si>
-    <t>Pembayaran Belanja Barang Sesuai Kwitansi Nomor:016/JSA.1/KW.SET BRSDM/I/2023 Tanggal 24 Januari 2023</t>
-  </si>
-  <si>
-    <t>'00052T</t>
-  </si>
-  <si>
-    <t>'00052A</t>
-  </si>
-  <si>
-    <t>Pembayaran Belanja Pegawai (Pembayaaran Tunjangan Kinerja PNS Set.BRSDM Bulan Januari 2023 Untuk 75 Pegawai)</t>
-  </si>
-  <si>
-    <t>'00057T</t>
-  </si>
-  <si>
-    <t>'07-FEB-23</t>
-  </si>
-  <si>
-    <t>'00057A</t>
-  </si>
-  <si>
-    <t>Pembyaran Belanja Barang Sesuai Surat TUgas  Nomor:B.304/BRSDM.1/KP.440/I/2023 Tanggal 10 Januari 2023</t>
-  </si>
-  <si>
-    <t>'00058T</t>
-  </si>
-  <si>
-    <t>'00058A</t>
-  </si>
-  <si>
-    <t>Pembayaran Belanja Barang Sesuai Surat Tugas Nomor:B.309/BRSDM.1/KP.440/I/2023 Tanggal 10 Januari 2023</t>
-  </si>
-  <si>
-    <t>'00059T</t>
-  </si>
-  <si>
-    <t>'08-FEB-23</t>
-  </si>
-  <si>
-    <t>Pembayaran Belanja Barang Sesuai Kwitansi Nomor:1300031276 Tanggal 30 Januari 2023</t>
+    <t>'00068T</t>
+  </si>
+  <si>
+    <t>10-FEB-23</t>
+  </si>
+  <si>
+    <t>'00068A</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Barang Berupa Honor PPNPN Bulan Januari Tahun 2023 untuk 1 Pegawai Sesuai Surat Keputusan Nomor:KEP.1/KPA/BRSDM/I/2023 Tanggal 02 Januari 2023</t>
+  </si>
+  <si>
+    <t>'00070T</t>
+  </si>
+  <si>
+    <t>'00070A</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Pegawai (Pembayaran Uang Makan PNS Pusdik Bulan Januari 2023 Untuk 41 Pegawai)</t>
+  </si>
+  <si>
+    <t>'00071T</t>
+  </si>
+  <si>
+    <t>'00071A</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Pegawai (Pembayaran Uang Makan PNS SET BRSDM Bulan Januari 2023 Untuk 72 Pegawai)</t>
+  </si>
+  <si>
+    <t>'00069T</t>
+  </si>
+  <si>
+    <t>'00069A</t>
+  </si>
+  <si>
+    <t>Pembayaran Belanja Pegawai (Pembayaran Uang Makan PNS Puslatluh Bulan Januari 2023 untuk 34 Pegawai)</t>
   </si>
 </sst>
 </file>
@@ -908,7 +1016,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:L112"/>
+  <dimension ref="A1:L122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="L3" sqref="L3"/>
@@ -1333,13 +1441,13 @@
         <v>17</v>
       </c>
       <c r="J13">
-        <v>511111</v>
+        <v>511126</v>
       </c>
       <c r="K13" t="s">
         <v>21</v>
       </c>
       <c r="L13">
-        <v>150882900</v>
+        <v>7966200</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1371,13 +1479,13 @@
         <v>17</v>
       </c>
       <c r="J14">
-        <v>511119</v>
+        <v>511125</v>
       </c>
       <c r="K14" t="s">
         <v>21</v>
       </c>
       <c r="L14">
-        <v>1642</v>
+        <v>457500</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -1409,13 +1517,13 @@
         <v>17</v>
       </c>
       <c r="J15">
-        <v>511121</v>
+        <v>511123</v>
       </c>
       <c r="K15" t="s">
         <v>21</v>
       </c>
       <c r="L15">
-        <v>10957550</v>
+        <v>3250000</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1429,13 +1537,13 @@
         <v>13</v>
       </c>
       <c r="D16" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E16" t="s">
         <v>15</v>
       </c>
       <c r="F16" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G16" t="s">
         <v>15</v>
@@ -1447,13 +1555,13 @@
         <v>17</v>
       </c>
       <c r="J16">
-        <v>511122</v>
+        <v>511151</v>
       </c>
       <c r="K16" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="L16">
-        <v>3340670</v>
+        <v>4800000</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -1467,13 +1575,13 @@
         <v>13</v>
       </c>
       <c r="D17" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E17" t="s">
         <v>15</v>
       </c>
       <c r="F17" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G17" t="s">
         <v>15</v>
@@ -1485,13 +1593,13 @@
         <v>17</v>
       </c>
       <c r="J17">
-        <v>511151</v>
+        <v>511126</v>
       </c>
       <c r="K17" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="L17">
-        <v>3150000</v>
+        <v>8690400</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -1505,13 +1613,13 @@
         <v>13</v>
       </c>
       <c r="D18" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E18" t="s">
         <v>15</v>
       </c>
       <c r="F18" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G18" t="s">
         <v>15</v>
@@ -1523,13 +1631,13 @@
         <v>17</v>
       </c>
       <c r="J18">
-        <v>511124</v>
+        <v>511125</v>
       </c>
       <c r="K18" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="L18">
-        <v>16590000</v>
+        <v>306071</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -1543,13 +1651,13 @@
         <v>13</v>
       </c>
       <c r="D19" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E19" t="s">
         <v>15</v>
       </c>
       <c r="F19" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G19" t="s">
         <v>15</v>
@@ -1561,13 +1669,13 @@
         <v>17</v>
       </c>
       <c r="J19">
-        <v>511126</v>
+        <v>511124</v>
       </c>
       <c r="K19" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="L19">
-        <v>7966200</v>
+        <v>11820000</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -1581,13 +1689,13 @@
         <v>13</v>
       </c>
       <c r="D20" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E20" t="s">
         <v>15</v>
       </c>
       <c r="F20" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G20" t="s">
         <v>15</v>
@@ -1599,13 +1707,13 @@
         <v>17</v>
       </c>
       <c r="J20">
-        <v>511125</v>
+        <v>511123</v>
       </c>
       <c r="K20" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="L20">
-        <v>457500</v>
+        <v>5770000</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -1619,13 +1727,13 @@
         <v>13</v>
       </c>
       <c r="D21" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E21" t="s">
         <v>15</v>
       </c>
       <c r="F21" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G21" t="s">
         <v>15</v>
@@ -1637,13 +1745,13 @@
         <v>17</v>
       </c>
       <c r="J21">
-        <v>511123</v>
+        <v>511122</v>
       </c>
       <c r="K21" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="L21">
-        <v>3250000</v>
+        <v>3273546</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -1675,13 +1783,13 @@
         <v>17</v>
       </c>
       <c r="J22">
-        <v>511151</v>
+        <v>511121</v>
       </c>
       <c r="K22" t="s">
         <v>24</v>
       </c>
       <c r="L22">
-        <v>4800000</v>
+        <v>10734680</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -1713,13 +1821,13 @@
         <v>17</v>
       </c>
       <c r="J23">
-        <v>511126</v>
+        <v>511111</v>
       </c>
       <c r="K23" t="s">
         <v>24</v>
       </c>
       <c r="L23">
-        <v>8690400</v>
+        <v>159350300</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -1751,13 +1859,13 @@
         <v>17</v>
       </c>
       <c r="J24">
-        <v>511125</v>
+        <v>511119</v>
       </c>
       <c r="K24" t="s">
         <v>24</v>
       </c>
       <c r="L24">
-        <v>306071</v>
+        <v>2349</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -1771,13 +1879,13 @@
         <v>13</v>
       </c>
       <c r="D25" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E25" t="s">
         <v>15</v>
       </c>
       <c r="F25" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G25" t="s">
         <v>15</v>
@@ -1789,13 +1897,13 @@
         <v>17</v>
       </c>
       <c r="J25">
-        <v>511124</v>
+        <v>511111</v>
       </c>
       <c r="K25" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="L25">
-        <v>11820000</v>
+        <v>150882900</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -1809,13 +1917,13 @@
         <v>13</v>
       </c>
       <c r="D26" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E26" t="s">
         <v>15</v>
       </c>
       <c r="F26" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G26" t="s">
         <v>15</v>
@@ -1827,13 +1935,13 @@
         <v>17</v>
       </c>
       <c r="J26">
-        <v>511123</v>
+        <v>511119</v>
       </c>
       <c r="K26" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="L26">
-        <v>5770000</v>
+        <v>1642</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -1847,13 +1955,13 @@
         <v>13</v>
       </c>
       <c r="D27" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E27" t="s">
         <v>15</v>
       </c>
       <c r="F27" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G27" t="s">
         <v>15</v>
@@ -1865,13 +1973,13 @@
         <v>17</v>
       </c>
       <c r="J27">
-        <v>511122</v>
+        <v>511121</v>
       </c>
       <c r="K27" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="L27">
-        <v>3273546</v>
+        <v>10957550</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -1885,13 +1993,13 @@
         <v>13</v>
       </c>
       <c r="D28" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E28" t="s">
         <v>15</v>
       </c>
       <c r="F28" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G28" t="s">
         <v>15</v>
@@ -1903,13 +2011,13 @@
         <v>17</v>
       </c>
       <c r="J28">
-        <v>511121</v>
+        <v>511122</v>
       </c>
       <c r="K28" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="L28">
-        <v>10734680</v>
+        <v>3340670</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -1923,13 +2031,13 @@
         <v>13</v>
       </c>
       <c r="D29" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E29" t="s">
         <v>15</v>
       </c>
       <c r="F29" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G29" t="s">
         <v>15</v>
@@ -1941,13 +2049,13 @@
         <v>17</v>
       </c>
       <c r="J29">
-        <v>511111</v>
+        <v>511151</v>
       </c>
       <c r="K29" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="L29">
-        <v>159350300</v>
+        <v>3150000</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -1961,13 +2069,13 @@
         <v>13</v>
       </c>
       <c r="D30" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E30" t="s">
         <v>15</v>
       </c>
       <c r="F30" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G30" t="s">
         <v>15</v>
@@ -1979,13 +2087,13 @@
         <v>17</v>
       </c>
       <c r="J30">
-        <v>511119</v>
+        <v>511124</v>
       </c>
       <c r="K30" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="L30">
-        <v>2349</v>
+        <v>16590000</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -2017,13 +2125,13 @@
         <v>17</v>
       </c>
       <c r="J31">
-        <v>511126</v>
+        <v>511119</v>
       </c>
       <c r="K31" t="s">
         <v>28</v>
       </c>
       <c r="L31">
-        <v>72420</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -2055,13 +2163,13 @@
         <v>17</v>
       </c>
       <c r="J32">
-        <v>511119</v>
+        <v>511111</v>
       </c>
       <c r="K32" t="s">
         <v>28</v>
       </c>
       <c r="L32">
-        <v>38</v>
+        <v>4151100</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -2093,13 +2201,13 @@
         <v>17</v>
       </c>
       <c r="J33">
-        <v>511111</v>
+        <v>511151</v>
       </c>
       <c r="K33" t="s">
         <v>28</v>
       </c>
       <c r="L33">
-        <v>4151100</v>
+        <v>190000</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -2131,13 +2239,13 @@
         <v>17</v>
       </c>
       <c r="J34">
-        <v>511151</v>
+        <v>511126</v>
       </c>
       <c r="K34" t="s">
         <v>28</v>
       </c>
       <c r="L34">
-        <v>190000</v>
+        <v>72420</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -2169,13 +2277,13 @@
         <v>17</v>
       </c>
       <c r="J35">
-        <v>511122</v>
+        <v>511111</v>
       </c>
       <c r="K35" t="s">
         <v>33</v>
       </c>
       <c r="L35">
-        <v>3278410</v>
+        <v>272938000</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -2207,13 +2315,13 @@
         <v>17</v>
       </c>
       <c r="J36">
-        <v>511123</v>
+        <v>511119</v>
       </c>
       <c r="K36" t="s">
         <v>33</v>
       </c>
       <c r="L36">
-        <v>5770000</v>
+        <v>3621</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -2245,13 +2353,13 @@
         <v>17</v>
       </c>
       <c r="J37">
-        <v>511124</v>
+        <v>511121</v>
       </c>
       <c r="K37" t="s">
         <v>33</v>
       </c>
       <c r="L37">
-        <v>11080000</v>
+        <v>16572730</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -2283,13 +2391,13 @@
         <v>17</v>
       </c>
       <c r="J38">
-        <v>511125</v>
+        <v>511122</v>
       </c>
       <c r="K38" t="s">
         <v>33</v>
       </c>
       <c r="L38">
-        <v>283271</v>
+        <v>5753906</v>
       </c>
     </row>
     <row r="39" spans="1:12">
@@ -2321,13 +2429,13 @@
         <v>17</v>
       </c>
       <c r="J39">
-        <v>511126</v>
+        <v>511151</v>
       </c>
       <c r="K39" t="s">
         <v>33</v>
       </c>
       <c r="L39">
-        <v>8690400</v>
+        <v>7560000</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -2359,13 +2467,13 @@
         <v>17</v>
       </c>
       <c r="J40">
-        <v>511151</v>
+        <v>511124</v>
       </c>
       <c r="K40" t="s">
         <v>33</v>
       </c>
       <c r="L40">
-        <v>4800000</v>
+        <v>23595000</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -2397,13 +2505,13 @@
         <v>17</v>
       </c>
       <c r="J41">
-        <v>511111</v>
+        <v>511125</v>
       </c>
       <c r="K41" t="s">
         <v>33</v>
       </c>
       <c r="L41">
-        <v>159625700</v>
+        <v>536569</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -2435,13 +2543,13 @@
         <v>17</v>
       </c>
       <c r="J42">
-        <v>511119</v>
+        <v>511126</v>
       </c>
       <c r="K42" t="s">
         <v>33</v>
       </c>
       <c r="L42">
-        <v>2446</v>
+        <v>14773680</v>
       </c>
     </row>
     <row r="43" spans="1:12">
@@ -2473,13 +2581,13 @@
         <v>17</v>
       </c>
       <c r="J43">
-        <v>511121</v>
+        <v>511123</v>
       </c>
       <c r="K43" t="s">
         <v>33</v>
       </c>
       <c r="L43">
-        <v>10754970</v>
+        <v>8750000</v>
       </c>
     </row>
     <row r="44" spans="1:12">
@@ -2511,13 +2619,13 @@
         <v>17</v>
       </c>
       <c r="J44">
-        <v>511126</v>
+        <v>511111</v>
       </c>
       <c r="K44" t="s">
         <v>36</v>
       </c>
       <c r="L44">
-        <v>14773680</v>
+        <v>159625700</v>
       </c>
     </row>
     <row r="45" spans="1:12">
@@ -2549,13 +2657,13 @@
         <v>17</v>
       </c>
       <c r="J45">
-        <v>511151</v>
+        <v>511119</v>
       </c>
       <c r="K45" t="s">
         <v>36</v>
       </c>
       <c r="L45">
-        <v>7560000</v>
+        <v>2446</v>
       </c>
     </row>
     <row r="46" spans="1:12">
@@ -2587,13 +2695,13 @@
         <v>17</v>
       </c>
       <c r="J46">
-        <v>511111</v>
+        <v>511121</v>
       </c>
       <c r="K46" t="s">
         <v>36</v>
       </c>
       <c r="L46">
-        <v>272938000</v>
+        <v>10754970</v>
       </c>
     </row>
     <row r="47" spans="1:12">
@@ -2625,13 +2733,13 @@
         <v>17</v>
       </c>
       <c r="J47">
-        <v>511119</v>
+        <v>511122</v>
       </c>
       <c r="K47" t="s">
         <v>36</v>
       </c>
       <c r="L47">
-        <v>3621</v>
+        <v>3278410</v>
       </c>
     </row>
     <row r="48" spans="1:12">
@@ -2663,13 +2771,13 @@
         <v>17</v>
       </c>
       <c r="J48">
-        <v>511121</v>
+        <v>511151</v>
       </c>
       <c r="K48" t="s">
         <v>36</v>
       </c>
       <c r="L48">
-        <v>16572730</v>
+        <v>4800000</v>
       </c>
     </row>
     <row r="49" spans="1:12">
@@ -2701,13 +2809,13 @@
         <v>17</v>
       </c>
       <c r="J49">
-        <v>511122</v>
+        <v>511124</v>
       </c>
       <c r="K49" t="s">
         <v>36</v>
       </c>
       <c r="L49">
-        <v>5753906</v>
+        <v>11080000</v>
       </c>
     </row>
     <row r="50" spans="1:12">
@@ -2739,13 +2847,13 @@
         <v>17</v>
       </c>
       <c r="J50">
-        <v>511123</v>
+        <v>511125</v>
       </c>
       <c r="K50" t="s">
         <v>36</v>
       </c>
       <c r="L50">
-        <v>8750000</v>
+        <v>283271</v>
       </c>
     </row>
     <row r="51" spans="1:12">
@@ -2777,13 +2885,13 @@
         <v>17</v>
       </c>
       <c r="J51">
-        <v>511124</v>
+        <v>511126</v>
       </c>
       <c r="K51" t="s">
         <v>36</v>
       </c>
       <c r="L51">
-        <v>23595000</v>
+        <v>8690400</v>
       </c>
     </row>
     <row r="52" spans="1:12">
@@ -2815,13 +2923,13 @@
         <v>17</v>
       </c>
       <c r="J52">
-        <v>511125</v>
+        <v>511123</v>
       </c>
       <c r="K52" t="s">
         <v>36</v>
       </c>
       <c r="L52">
-        <v>536569</v>
+        <v>5770000</v>
       </c>
     </row>
     <row r="53" spans="1:12">
@@ -2853,13 +2961,13 @@
         <v>17</v>
       </c>
       <c r="J53">
-        <v>511119</v>
+        <v>511111</v>
       </c>
       <c r="K53" t="s">
         <v>39</v>
       </c>
       <c r="L53">
-        <v>1640</v>
+        <v>151536800</v>
       </c>
     </row>
     <row r="54" spans="1:12">
@@ -2891,13 +2999,13 @@
         <v>17</v>
       </c>
       <c r="J54">
-        <v>511111</v>
+        <v>511119</v>
       </c>
       <c r="K54" t="s">
         <v>39</v>
       </c>
       <c r="L54">
-        <v>151536800</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="55" spans="1:12">
@@ -2929,13 +3037,13 @@
         <v>17</v>
       </c>
       <c r="J55">
-        <v>511151</v>
+        <v>511121</v>
       </c>
       <c r="K55" t="s">
         <v>39</v>
       </c>
       <c r="L55">
-        <v>3150000</v>
+        <v>10982140</v>
       </c>
     </row>
     <row r="56" spans="1:12">
@@ -2967,13 +3075,13 @@
         <v>17</v>
       </c>
       <c r="J56">
-        <v>511121</v>
+        <v>511122</v>
       </c>
       <c r="K56" t="s">
         <v>39</v>
       </c>
       <c r="L56">
-        <v>10982140</v>
+        <v>3358666</v>
       </c>
     </row>
     <row r="57" spans="1:12">
@@ -3005,13 +3113,13 @@
         <v>17</v>
       </c>
       <c r="J57">
-        <v>511122</v>
+        <v>511151</v>
       </c>
       <c r="K57" t="s">
         <v>39</v>
       </c>
       <c r="L57">
-        <v>3358666</v>
+        <v>3150000</v>
       </c>
     </row>
     <row r="58" spans="1:12">
@@ -3043,13 +3151,13 @@
         <v>17</v>
       </c>
       <c r="J58">
-        <v>511123</v>
+        <v>511124</v>
       </c>
       <c r="K58" t="s">
         <v>39</v>
       </c>
       <c r="L58">
-        <v>3250000</v>
+        <v>15850000</v>
       </c>
     </row>
     <row r="59" spans="1:12">
@@ -3081,13 +3189,13 @@
         <v>17</v>
       </c>
       <c r="J59">
-        <v>511124</v>
+        <v>511125</v>
       </c>
       <c r="K59" t="s">
         <v>39</v>
       </c>
       <c r="L59">
-        <v>15850000</v>
+        <v>434700</v>
       </c>
     </row>
     <row r="60" spans="1:12">
@@ -3119,13 +3227,13 @@
         <v>17</v>
       </c>
       <c r="J60">
-        <v>511125</v>
+        <v>511126</v>
       </c>
       <c r="K60" t="s">
         <v>39</v>
       </c>
       <c r="L60">
-        <v>434700</v>
+        <v>7966200</v>
       </c>
     </row>
     <row r="61" spans="1:12">
@@ -3157,13 +3265,13 @@
         <v>17</v>
       </c>
       <c r="J61">
-        <v>511126</v>
+        <v>511123</v>
       </c>
       <c r="K61" t="s">
         <v>39</v>
       </c>
       <c r="L61">
-        <v>7966200</v>
+        <v>3250000</v>
       </c>
     </row>
     <row r="62" spans="1:12">
@@ -3186,7 +3294,7 @@
         <v>42</v>
       </c>
       <c r="G62" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="H62">
         <v>2378</v>
@@ -3195,13 +3303,13 @@
         <v>17</v>
       </c>
       <c r="J62">
-        <v>522111</v>
+        <v>521111</v>
       </c>
       <c r="K62" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="L62">
-        <v>149880784</v>
+        <v>66800000</v>
       </c>
     </row>
     <row r="63" spans="1:12">
@@ -3215,16 +3323,16 @@
         <v>13</v>
       </c>
       <c r="D63" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E63" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F63" t="s">
         <v>46</v>
       </c>
       <c r="G63" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="H63">
         <v>2378</v>
@@ -3233,13 +3341,13 @@
         <v>17</v>
       </c>
       <c r="J63">
-        <v>522113</v>
+        <v>522111</v>
       </c>
       <c r="K63" t="s">
         <v>47</v>
       </c>
       <c r="L63">
-        <v>12252499</v>
+        <v>149880784</v>
       </c>
     </row>
     <row r="64" spans="1:12">
@@ -3256,14 +3364,14 @@
         <v>48</v>
       </c>
       <c r="E64" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="F64" t="s">
+        <v>50</v>
+      </c>
+      <c r="G64" t="s">
         <v>49</v>
       </c>
-      <c r="G64" t="s">
-        <v>50</v>
-      </c>
       <c r="H64">
         <v>2378</v>
       </c>
@@ -3271,13 +3379,13 @@
         <v>17</v>
       </c>
       <c r="J64">
-        <v>521111</v>
+        <v>522113</v>
       </c>
       <c r="K64" t="s">
         <v>51</v>
       </c>
       <c r="L64">
-        <v>66800000</v>
+        <v>12252499</v>
       </c>
     </row>
     <row r="65" spans="1:12">
@@ -3294,28 +3402,28 @@
         <v>52</v>
       </c>
       <c r="E65" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F65" t="s">
         <v>53</v>
       </c>
       <c r="G65" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H65">
         <v>2378</v>
       </c>
       <c r="I65" t="s">
+        <v>17</v>
+      </c>
+      <c r="J65">
+        <v>521111</v>
+      </c>
+      <c r="K65" t="s">
         <v>54</v>
       </c>
-      <c r="J65">
-        <v>524114</v>
-      </c>
-      <c r="K65" t="s">
-        <v>55</v>
-      </c>
       <c r="L65">
-        <v>300000</v>
+        <v>206715000</v>
       </c>
     </row>
     <row r="66" spans="1:12">
@@ -3329,31 +3437,31 @@
         <v>13</v>
       </c>
       <c r="D66" t="s">
+        <v>55</v>
+      </c>
+      <c r="E66" t="s">
+        <v>49</v>
+      </c>
+      <c r="F66" t="s">
         <v>56</v>
       </c>
-      <c r="E66" t="s">
-        <v>50</v>
-      </c>
-      <c r="F66" t="s">
+      <c r="G66" t="s">
+        <v>43</v>
+      </c>
+      <c r="H66">
+        <v>2378</v>
+      </c>
+      <c r="I66" t="s">
+        <v>17</v>
+      </c>
+      <c r="J66">
+        <v>521111</v>
+      </c>
+      <c r="K66" t="s">
         <v>57</v>
       </c>
-      <c r="G66" t="s">
-        <v>50</v>
-      </c>
-      <c r="H66">
-        <v>2378</v>
-      </c>
-      <c r="I66" t="s">
-        <v>17</v>
-      </c>
-      <c r="J66">
-        <v>524111</v>
-      </c>
-      <c r="K66" t="s">
-        <v>58</v>
-      </c>
       <c r="L66">
-        <v>19900000</v>
+        <v>82100000</v>
       </c>
     </row>
     <row r="67" spans="1:12">
@@ -3367,22 +3475,22 @@
         <v>13</v>
       </c>
       <c r="D67" t="s">
+        <v>58</v>
+      </c>
+      <c r="E67" t="s">
+        <v>43</v>
+      </c>
+      <c r="F67" t="s">
         <v>59</v>
       </c>
-      <c r="E67" t="s">
-        <v>50</v>
-      </c>
-      <c r="F67" t="s">
+      <c r="G67" t="s">
+        <v>43</v>
+      </c>
+      <c r="H67">
+        <v>2378</v>
+      </c>
+      <c r="I67" t="s">
         <v>60</v>
-      </c>
-      <c r="G67" t="s">
-        <v>50</v>
-      </c>
-      <c r="H67">
-        <v>2378</v>
-      </c>
-      <c r="I67" t="s">
-        <v>54</v>
       </c>
       <c r="J67">
         <v>524111</v>
@@ -3391,7 +3499,7 @@
         <v>61</v>
       </c>
       <c r="L67">
-        <v>720000</v>
+        <v>20738160</v>
       </c>
     </row>
     <row r="68" spans="1:12">
@@ -3408,28 +3516,28 @@
         <v>62</v>
       </c>
       <c r="E68" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="F68" t="s">
         <v>63</v>
       </c>
       <c r="G68" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="H68">
         <v>2378</v>
       </c>
       <c r="I68" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="J68">
         <v>524111</v>
       </c>
       <c r="K68" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="L68">
-        <v>20738160</v>
+        <v>1334500</v>
       </c>
     </row>
     <row r="69" spans="1:12">
@@ -3443,16 +3551,16 @@
         <v>13</v>
       </c>
       <c r="D69" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E69" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="F69" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G69" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="H69">
         <v>2378</v>
@@ -3464,10 +3572,10 @@
         <v>524111</v>
       </c>
       <c r="K69" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="L69">
-        <v>1334500</v>
+        <v>45645400</v>
       </c>
     </row>
     <row r="70" spans="1:12">
@@ -3481,31 +3589,31 @@
         <v>13</v>
       </c>
       <c r="D70" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E70" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F70" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G70" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H70">
         <v>2378</v>
       </c>
       <c r="I70" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
       <c r="J70">
-        <v>521111</v>
+        <v>524111</v>
       </c>
       <c r="K70" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="L70">
-        <v>206715000</v>
+        <v>15082960</v>
       </c>
     </row>
     <row r="71" spans="1:12">
@@ -3522,13 +3630,13 @@
         <v>70</v>
       </c>
       <c r="E71" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F71" t="s">
         <v>71</v>
       </c>
       <c r="G71" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="H71">
         <v>2378</v>
@@ -3537,13 +3645,13 @@
         <v>17</v>
       </c>
       <c r="J71">
-        <v>521111</v>
+        <v>524111</v>
       </c>
       <c r="K71" t="s">
         <v>72</v>
       </c>
       <c r="L71">
-        <v>82100000</v>
+        <v>21841204</v>
       </c>
     </row>
     <row r="72" spans="1:12">
@@ -3560,28 +3668,28 @@
         <v>73</v>
       </c>
       <c r="E72" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="F72" t="s">
         <v>74</v>
       </c>
       <c r="G72" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="H72">
         <v>2378</v>
       </c>
       <c r="I72" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="J72">
-        <v>524111</v>
+        <v>524119</v>
       </c>
       <c r="K72" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="L72">
-        <v>15082960</v>
+        <v>1152800</v>
       </c>
     </row>
     <row r="73" spans="1:12">
@@ -3595,16 +3703,16 @@
         <v>13</v>
       </c>
       <c r="D73" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E73" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="F73" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G73" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="H73">
         <v>2378</v>
@@ -3613,13 +3721,13 @@
         <v>17</v>
       </c>
       <c r="J73">
-        <v>524111</v>
+        <v>524114</v>
       </c>
       <c r="K73" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="L73">
-        <v>21841204</v>
+        <v>820000</v>
       </c>
     </row>
     <row r="74" spans="1:12">
@@ -3633,31 +3741,31 @@
         <v>13</v>
       </c>
       <c r="D74" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E74" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="F74" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G74" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="H74">
         <v>2378</v>
       </c>
       <c r="I74" t="s">
-        <v>54</v>
+        <v>81</v>
       </c>
       <c r="J74">
-        <v>524119</v>
+        <v>524111</v>
       </c>
       <c r="K74" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="L74">
-        <v>1152800</v>
+        <v>93138974</v>
       </c>
     </row>
     <row r="75" spans="1:12">
@@ -3671,31 +3779,31 @@
         <v>13</v>
       </c>
       <c r="D75" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E75" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="F75" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G75" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="H75">
         <v>2378</v>
       </c>
       <c r="I75" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
       <c r="J75">
         <v>524114</v>
       </c>
       <c r="K75" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="L75">
-        <v>820000</v>
+        <v>300000</v>
       </c>
     </row>
     <row r="76" spans="1:12">
@@ -3709,31 +3817,31 @@
         <v>13</v>
       </c>
       <c r="D76" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E76" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="F76" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G76" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="H76">
         <v>2378</v>
       </c>
       <c r="I76" t="s">
-        <v>86</v>
+        <v>17</v>
       </c>
       <c r="J76">
         <v>524111</v>
       </c>
       <c r="K76" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="L76">
-        <v>93138974</v>
+        <v>19900000</v>
       </c>
     </row>
     <row r="77" spans="1:12">
@@ -3750,19 +3858,19 @@
         <v>87</v>
       </c>
       <c r="E77" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="F77" t="s">
         <v>88</v>
       </c>
       <c r="G77" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="H77">
         <v>2378</v>
       </c>
       <c r="I77" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
       <c r="J77">
         <v>524111</v>
@@ -3771,7 +3879,7 @@
         <v>89</v>
       </c>
       <c r="L77">
-        <v>45645400</v>
+        <v>720000</v>
       </c>
     </row>
     <row r="78" spans="1:12">
@@ -3832,22 +3940,22 @@
         <v>96</v>
       </c>
       <c r="G79" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H79">
         <v>2378</v>
       </c>
       <c r="I79" t="s">
-        <v>17</v>
+        <v>81</v>
       </c>
       <c r="J79">
-        <v>524111</v>
+        <v>522191</v>
       </c>
       <c r="K79" t="s">
         <v>97</v>
       </c>
       <c r="L79">
-        <v>50692502</v>
+        <v>195000000</v>
       </c>
     </row>
     <row r="80" spans="1:12">
@@ -3870,22 +3978,22 @@
         <v>99</v>
       </c>
       <c r="G80" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="H80">
         <v>2378</v>
       </c>
       <c r="I80" t="s">
-        <v>86</v>
+        <v>17</v>
       </c>
       <c r="J80">
-        <v>522191</v>
+        <v>524111</v>
       </c>
       <c r="K80" t="s">
         <v>100</v>
       </c>
       <c r="L80">
-        <v>195000000</v>
+        <v>50692502</v>
       </c>
     </row>
     <row r="81" spans="1:12">
@@ -3902,28 +4010,28 @@
         <v>101</v>
       </c>
       <c r="E81" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="F81" t="s">
+        <v>103</v>
+      </c>
+      <c r="G81" t="s">
         <v>102</v>
       </c>
-      <c r="G81" t="s">
-        <v>93</v>
-      </c>
       <c r="H81">
         <v>2378</v>
       </c>
       <c r="I81" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="J81">
         <v>524111</v>
       </c>
       <c r="K81" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="L81">
-        <v>8591000</v>
+        <v>9753677</v>
       </c>
     </row>
     <row r="82" spans="1:12">
@@ -3937,31 +4045,31 @@
         <v>13</v>
       </c>
       <c r="D82" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E82" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F82" t="s">
         <v>106</v>
       </c>
       <c r="G82" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="H82">
         <v>2378</v>
       </c>
       <c r="I82" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="J82">
-        <v>524111</v>
+        <v>522151</v>
       </c>
       <c r="K82" t="s">
         <v>107</v>
       </c>
       <c r="L82">
-        <v>320961489</v>
+        <v>1800000</v>
       </c>
     </row>
     <row r="83" spans="1:12">
@@ -3978,25 +4086,25 @@
         <v>108</v>
       </c>
       <c r="E83" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="F83" t="s">
+        <v>110</v>
+      </c>
+      <c r="G83" t="s">
         <v>109</v>
       </c>
-      <c r="G83" t="s">
-        <v>105</v>
-      </c>
       <c r="H83">
         <v>2378</v>
       </c>
       <c r="I83" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="J83">
         <v>521211</v>
       </c>
       <c r="K83" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="L83">
         <v>38500000</v>
@@ -4013,13 +4121,13 @@
         <v>13</v>
       </c>
       <c r="D84" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E84" t="s">
         <v>93</v>
       </c>
       <c r="F84" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G84" t="s">
         <v>93</v>
@@ -4028,13 +4136,13 @@
         <v>2378</v>
       </c>
       <c r="I84" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="J84">
         <v>524111</v>
       </c>
       <c r="K84" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="L84">
         <v>16821479</v>
@@ -4051,31 +4159,31 @@
         <v>13</v>
       </c>
       <c r="D85" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E85" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="F85" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G85" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="H85">
         <v>2378</v>
       </c>
       <c r="I85" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="J85">
-        <v>521211</v>
+        <v>524111</v>
       </c>
       <c r="K85" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="L85">
-        <v>41208750</v>
+        <v>320961489</v>
       </c>
     </row>
     <row r="86" spans="1:12">
@@ -4089,31 +4197,31 @@
         <v>13</v>
       </c>
       <c r="D86" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E86" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="F86" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G86" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="H86">
         <v>2378</v>
       </c>
       <c r="I86" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="J86">
         <v>524111</v>
       </c>
       <c r="K86" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="L86">
-        <v>5326766</v>
+        <v>8591000</v>
       </c>
     </row>
     <row r="87" spans="1:12">
@@ -4127,31 +4235,31 @@
         <v>13</v>
       </c>
       <c r="D87" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E87" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="F87" t="s">
         <v>122</v>
       </c>
       <c r="G87" t="s">
+        <v>109</v>
+      </c>
+      <c r="H87">
+        <v>2378</v>
+      </c>
+      <c r="I87" t="s">
+        <v>60</v>
+      </c>
+      <c r="J87">
+        <v>524111</v>
+      </c>
+      <c r="K87" t="s">
         <v>123</v>
       </c>
-      <c r="H87">
-        <v>2378</v>
-      </c>
-      <c r="I87" t="s">
-        <v>17</v>
-      </c>
-      <c r="J87">
-        <v>522191</v>
-      </c>
-      <c r="K87" t="s">
-        <v>124</v>
-      </c>
       <c r="L87">
-        <v>37249665</v>
+        <v>5326766</v>
       </c>
     </row>
     <row r="88" spans="1:12">
@@ -4165,31 +4273,31 @@
         <v>13</v>
       </c>
       <c r="D88" t="s">
+        <v>124</v>
+      </c>
+      <c r="E88" t="s">
+        <v>109</v>
+      </c>
+      <c r="F88" t="s">
         <v>125</v>
       </c>
-      <c r="E88" t="s">
-        <v>121</v>
-      </c>
-      <c r="F88" t="s">
+      <c r="G88" t="s">
+        <v>109</v>
+      </c>
+      <c r="H88">
+        <v>2378</v>
+      </c>
+      <c r="I88" t="s">
+        <v>60</v>
+      </c>
+      <c r="J88">
+        <v>521211</v>
+      </c>
+      <c r="K88" t="s">
         <v>126</v>
       </c>
-      <c r="G88" t="s">
-        <v>123</v>
-      </c>
-      <c r="H88">
-        <v>2378</v>
-      </c>
-      <c r="I88" t="s">
-        <v>17</v>
-      </c>
-      <c r="J88">
-        <v>522191</v>
-      </c>
-      <c r="K88" t="s">
-        <v>127</v>
-      </c>
       <c r="L88">
-        <v>37368335</v>
+        <v>41208750</v>
       </c>
     </row>
     <row r="89" spans="1:12">
@@ -4203,16 +4311,16 @@
         <v>13</v>
       </c>
       <c r="D89" t="s">
+        <v>127</v>
+      </c>
+      <c r="E89" t="s">
         <v>128</v>
-      </c>
-      <c r="E89" t="s">
-        <v>121</v>
       </c>
       <c r="F89" t="s">
         <v>129</v>
       </c>
       <c r="G89" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="H89">
         <v>2378</v>
@@ -4221,13 +4329,13 @@
         <v>17</v>
       </c>
       <c r="J89">
-        <v>524111</v>
+        <v>522191</v>
       </c>
       <c r="K89" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="L89">
-        <v>9800000</v>
+        <v>37249665</v>
       </c>
     </row>
     <row r="90" spans="1:12">
@@ -4241,16 +4349,16 @@
         <v>13</v>
       </c>
       <c r="D90" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E90" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F90" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G90" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="H90">
         <v>2378</v>
@@ -4259,13 +4367,13 @@
         <v>17</v>
       </c>
       <c r="J90">
-        <v>524111</v>
+        <v>522191</v>
       </c>
       <c r="K90" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="L90">
-        <v>7140000</v>
+        <v>37368335</v>
       </c>
     </row>
     <row r="91" spans="1:12">
@@ -4279,31 +4387,31 @@
         <v>13</v>
       </c>
       <c r="D91" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E91" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F91" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G91" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="H91">
         <v>2378</v>
       </c>
       <c r="I91" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="J91">
         <v>524111</v>
       </c>
       <c r="K91" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="L91">
-        <v>4590000</v>
+        <v>9800000</v>
       </c>
     </row>
     <row r="92" spans="1:12">
@@ -4317,16 +4425,16 @@
         <v>13</v>
       </c>
       <c r="D92" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E92" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="F92" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G92" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="H92">
         <v>2378</v>
@@ -4338,10 +4446,10 @@
         <v>524111</v>
       </c>
       <c r="K92" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="L92">
-        <v>6775500</v>
+        <v>7140000</v>
       </c>
     </row>
     <row r="93" spans="1:12">
@@ -4355,31 +4463,31 @@
         <v>13</v>
       </c>
       <c r="D93" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E93" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="F93" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G93" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="H93">
         <v>2378</v>
       </c>
       <c r="I93" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
       <c r="J93">
         <v>524111</v>
       </c>
       <c r="K93" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="L93">
-        <v>8468650</v>
+        <v>4590000</v>
       </c>
     </row>
     <row r="94" spans="1:12">
@@ -4393,16 +4501,16 @@
         <v>13</v>
       </c>
       <c r="D94" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E94" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="F94" t="s">
         <v>145</v>
       </c>
       <c r="G94" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="H94">
         <v>2378</v>
@@ -4411,13 +4519,13 @@
         <v>17</v>
       </c>
       <c r="J94">
-        <v>511124</v>
+        <v>524111</v>
       </c>
       <c r="K94" t="s">
         <v>146</v>
       </c>
       <c r="L94">
-        <v>114960000</v>
+        <v>8468650</v>
       </c>
     </row>
     <row r="95" spans="1:12">
@@ -4431,16 +4539,16 @@
         <v>13</v>
       </c>
       <c r="D95" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="E95" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="F95" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="G95" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="H95">
         <v>2378</v>
@@ -4449,13 +4557,13 @@
         <v>17</v>
       </c>
       <c r="J95">
-        <v>511125</v>
+        <v>524111</v>
       </c>
       <c r="K95" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="L95">
-        <v>2050</v>
+        <v>6775500</v>
       </c>
     </row>
     <row r="96" spans="1:12">
@@ -4469,16 +4577,16 @@
         <v>13</v>
       </c>
       <c r="D96" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="E96" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="F96" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="G96" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="H96">
         <v>2378</v>
@@ -4487,13 +4595,13 @@
         <v>17</v>
       </c>
       <c r="J96">
-        <v>511119</v>
+        <v>511124</v>
       </c>
       <c r="K96" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="L96">
-        <v>1900</v>
+        <v>91040000</v>
       </c>
     </row>
     <row r="97" spans="1:12">
@@ -4507,16 +4615,16 @@
         <v>13</v>
       </c>
       <c r="D97" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="E97" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="F97" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="G97" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="H97">
         <v>2378</v>
@@ -4528,10 +4636,10 @@
         <v>511124</v>
       </c>
       <c r="K97" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="L97">
-        <v>75400000</v>
+        <v>114960000</v>
       </c>
     </row>
     <row r="98" spans="1:12">
@@ -4545,16 +4653,16 @@
         <v>13</v>
       </c>
       <c r="D98" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="E98" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="F98" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="G98" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="H98">
         <v>2378</v>
@@ -4566,10 +4674,10 @@
         <v>511125</v>
       </c>
       <c r="K98" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="L98">
-        <v>265210</v>
+        <v>2050</v>
       </c>
     </row>
     <row r="99" spans="1:12">
@@ -4583,17 +4691,17 @@
         <v>13</v>
       </c>
       <c r="D99" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="E99" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="F99" t="s">
+        <v>158</v>
+      </c>
+      <c r="G99" t="s">
         <v>151</v>
       </c>
-      <c r="G99" t="s">
-        <v>144</v>
-      </c>
       <c r="H99">
         <v>2378</v>
       </c>
@@ -4601,13 +4709,13 @@
         <v>17</v>
       </c>
       <c r="J99">
-        <v>511124</v>
+        <v>511119</v>
       </c>
       <c r="K99" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="L99">
-        <v>91040000</v>
+        <v>1900</v>
       </c>
     </row>
     <row r="100" spans="1:12">
@@ -4621,16 +4729,16 @@
         <v>13</v>
       </c>
       <c r="D100" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="E100" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="F100" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="G100" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="H100">
         <v>2378</v>
@@ -4639,13 +4747,13 @@
         <v>17</v>
       </c>
       <c r="J100">
-        <v>511111</v>
+        <v>511124</v>
       </c>
       <c r="K100" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="L100">
-        <v>7036200</v>
+        <v>75400000</v>
       </c>
     </row>
     <row r="101" spans="1:12">
@@ -4659,16 +4767,16 @@
         <v>13</v>
       </c>
       <c r="D101" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="E101" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="F101" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="G101" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="H101">
         <v>2378</v>
@@ -4677,13 +4785,13 @@
         <v>17</v>
       </c>
       <c r="J101">
-        <v>511119</v>
+        <v>511125</v>
       </c>
       <c r="K101" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="L101">
-        <v>36</v>
+        <v>265210</v>
       </c>
     </row>
     <row r="102" spans="1:12">
@@ -4697,16 +4805,16 @@
         <v>13</v>
       </c>
       <c r="D102" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="E102" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="F102" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="G102" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="H102">
         <v>2378</v>
@@ -4715,13 +4823,13 @@
         <v>17</v>
       </c>
       <c r="J102">
-        <v>511126</v>
+        <v>511111</v>
       </c>
       <c r="K102" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="L102">
-        <v>144840</v>
+        <v>7036200</v>
       </c>
     </row>
     <row r="103" spans="1:12">
@@ -4735,16 +4843,16 @@
         <v>13</v>
       </c>
       <c r="D103" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="E103" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="F103" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="G103" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="H103">
         <v>2378</v>
@@ -4753,13 +4861,13 @@
         <v>17</v>
       </c>
       <c r="J103">
-        <v>511151</v>
+        <v>511119</v>
       </c>
       <c r="K103" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="L103">
-        <v>370000</v>
+        <v>36</v>
       </c>
     </row>
     <row r="104" spans="1:12">
@@ -4773,13 +4881,17 @@
         <v>13</v>
       </c>
       <c r="D104" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="E104" t="s">
-        <v>157</v>
-      </c>
-      <c r="F104"/>
-      <c r="G104"/>
+        <v>151</v>
+      </c>
+      <c r="F104" t="s">
+        <v>161</v>
+      </c>
+      <c r="G104" t="s">
+        <v>151</v>
+      </c>
       <c r="H104">
         <v>2378</v>
       </c>
@@ -4787,13 +4899,13 @@
         <v>17</v>
       </c>
       <c r="J104">
-        <v>521111</v>
+        <v>511126</v>
       </c>
       <c r="K104" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="L104">
-        <v>10208000</v>
+        <v>144840</v>
       </c>
     </row>
     <row r="105" spans="1:12">
@@ -4807,16 +4919,16 @@
         <v>13</v>
       </c>
       <c r="D105" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E105" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="F105" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="G105" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="H105">
         <v>2378</v>
@@ -4825,13 +4937,13 @@
         <v>17</v>
       </c>
       <c r="J105">
-        <v>524111</v>
+        <v>511151</v>
       </c>
       <c r="K105" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="L105">
-        <v>7370735</v>
+        <v>370000</v>
       </c>
     </row>
     <row r="106" spans="1:12">
@@ -4845,16 +4957,16 @@
         <v>13</v>
       </c>
       <c r="D106" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E106" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="F106" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="G106" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="H106">
         <v>2378</v>
@@ -4866,7 +4978,7 @@
         <v>512411</v>
       </c>
       <c r="K106" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="L106">
         <v>204565986</v>
@@ -4883,31 +4995,31 @@
         <v>13</v>
       </c>
       <c r="D107" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="E107" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="F107" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="G107" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="H107">
         <v>2378</v>
       </c>
       <c r="I107" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
       <c r="J107">
-        <v>512411</v>
+        <v>521211</v>
       </c>
       <c r="K107" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="L107">
-        <v>228513450</v>
+        <v>24500000</v>
       </c>
     </row>
     <row r="108" spans="1:12">
@@ -4921,31 +5033,31 @@
         <v>13</v>
       </c>
       <c r="D108" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="E108" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="F108" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="G108" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="H108">
         <v>2378</v>
       </c>
       <c r="I108" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="J108">
-        <v>521211</v>
+        <v>512411</v>
       </c>
       <c r="K108" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="L108">
-        <v>24500000</v>
+        <v>411490206</v>
       </c>
     </row>
     <row r="109" spans="1:12">
@@ -4959,16 +5071,16 @@
         <v>13</v>
       </c>
       <c r="D109" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E109" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="F109" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="G109" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="H109">
         <v>2378</v>
@@ -4977,13 +5089,13 @@
         <v>17</v>
       </c>
       <c r="J109">
-        <v>512411</v>
+        <v>524111</v>
       </c>
       <c r="K109" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="L109">
-        <v>411490206</v>
+        <v>7370735</v>
       </c>
     </row>
     <row r="110" spans="1:12">
@@ -4997,16 +5109,16 @@
         <v>13</v>
       </c>
       <c r="D110" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="E110" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="F110" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="G110" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="H110">
         <v>2378</v>
@@ -5015,13 +5127,13 @@
         <v>17</v>
       </c>
       <c r="J110">
-        <v>524111</v>
+        <v>512411</v>
       </c>
       <c r="K110" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="L110">
-        <v>9753677</v>
+        <v>228513450</v>
       </c>
     </row>
     <row r="111" spans="1:12">
@@ -5035,31 +5147,31 @@
         <v>13</v>
       </c>
       <c r="D111" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E111" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="F111" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="G111" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="H111">
         <v>2378</v>
       </c>
       <c r="I111" t="s">
-        <v>17</v>
+        <v>182</v>
       </c>
       <c r="J111">
-        <v>522151</v>
+        <v>532111</v>
       </c>
       <c r="K111" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="L111">
-        <v>1800000</v>
+        <v>510700000</v>
       </c>
     </row>
     <row r="112" spans="1:12">
@@ -5073,27 +5185,411 @@
         <v>13</v>
       </c>
       <c r="D112" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="E112" t="s">
+        <v>180</v>
+      </c>
+      <c r="F112" t="s">
+        <v>185</v>
+      </c>
+      <c r="G112" t="s">
+        <v>186</v>
+      </c>
+      <c r="H112">
+        <v>4345</v>
+      </c>
+      <c r="I112" t="s">
+        <v>81</v>
+      </c>
+      <c r="J112">
+        <v>521219</v>
+      </c>
+      <c r="K112" t="s">
+        <v>187</v>
+      </c>
+      <c r="L112">
+        <v>232550040</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12">
+      <c r="A113">
+        <v>110</v>
+      </c>
+      <c r="B113">
+        <v>626402</v>
+      </c>
+      <c r="C113" t="s">
+        <v>13</v>
+      </c>
+      <c r="D113" t="s">
+        <v>188</v>
+      </c>
+      <c r="E113" t="s">
+        <v>180</v>
+      </c>
+      <c r="F113" t="s">
+        <v>189</v>
+      </c>
+      <c r="G113" t="s">
+        <v>186</v>
+      </c>
+      <c r="H113">
+        <v>4345</v>
+      </c>
+      <c r="I113" t="s">
+        <v>81</v>
+      </c>
+      <c r="J113">
+        <v>521219</v>
+      </c>
+      <c r="K113" t="s">
+        <v>190</v>
+      </c>
+      <c r="L113">
+        <v>138195036</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12">
+      <c r="A114">
+        <v>111</v>
+      </c>
+      <c r="B114">
+        <v>626402</v>
+      </c>
+      <c r="C114" t="s">
+        <v>13</v>
+      </c>
+      <c r="D114" t="s">
+        <v>191</v>
+      </c>
+      <c r="E114" t="s">
+        <v>180</v>
+      </c>
+      <c r="F114" t="s">
+        <v>192</v>
+      </c>
+      <c r="G114" t="s">
+        <v>180</v>
+      </c>
+      <c r="H114">
+        <v>2378</v>
+      </c>
+      <c r="I114" t="s">
+        <v>17</v>
+      </c>
+      <c r="J114">
+        <v>523121</v>
+      </c>
+      <c r="K114" t="s">
+        <v>193</v>
+      </c>
+      <c r="L114">
+        <v>9751000</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12">
+      <c r="A115">
+        <v>112</v>
+      </c>
+      <c r="B115">
+        <v>626402</v>
+      </c>
+      <c r="C115" t="s">
+        <v>13</v>
+      </c>
+      <c r="D115" t="s">
+        <v>194</v>
+      </c>
+      <c r="E115" t="s">
+        <v>180</v>
+      </c>
+      <c r="F115" t="s">
+        <v>195</v>
+      </c>
+      <c r="G115" t="s">
+        <v>180</v>
+      </c>
+      <c r="H115">
+        <v>2378</v>
+      </c>
+      <c r="I115" t="s">
         <v>182</v>
       </c>
-      <c r="F112"/>
-      <c r="G112"/>
-      <c r="H112">
-        <v>2378</v>
-      </c>
-      <c r="I112" t="s">
-        <v>17</v>
-      </c>
-      <c r="J112">
-        <v>522119</v>
-      </c>
-      <c r="K112" t="s">
-        <v>183</v>
-      </c>
-      <c r="L112">
-        <v>21756000</v>
+      <c r="J115">
+        <v>532111</v>
+      </c>
+      <c r="K115" t="s">
+        <v>196</v>
+      </c>
+      <c r="L115">
+        <v>115820000</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12">
+      <c r="A116">
+        <v>113</v>
+      </c>
+      <c r="B116">
+        <v>626402</v>
+      </c>
+      <c r="C116" t="s">
+        <v>13</v>
+      </c>
+      <c r="D116" t="s">
+        <v>197</v>
+      </c>
+      <c r="E116" t="s">
+        <v>180</v>
+      </c>
+      <c r="F116" t="s">
+        <v>198</v>
+      </c>
+      <c r="G116" t="s">
+        <v>186</v>
+      </c>
+      <c r="H116">
+        <v>2378</v>
+      </c>
+      <c r="I116" t="s">
+        <v>17</v>
+      </c>
+      <c r="J116">
+        <v>524111</v>
+      </c>
+      <c r="K116" t="s">
+        <v>199</v>
+      </c>
+      <c r="L116">
+        <v>16394000</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12">
+      <c r="A117">
+        <v>114</v>
+      </c>
+      <c r="B117">
+        <v>626402</v>
+      </c>
+      <c r="C117" t="s">
+        <v>13</v>
+      </c>
+      <c r="D117" t="s">
+        <v>200</v>
+      </c>
+      <c r="E117" t="s">
+        <v>180</v>
+      </c>
+      <c r="F117" t="s">
+        <v>201</v>
+      </c>
+      <c r="G117" t="s">
+        <v>180</v>
+      </c>
+      <c r="H117">
+        <v>2378</v>
+      </c>
+      <c r="I117" t="s">
+        <v>17</v>
+      </c>
+      <c r="J117">
+        <v>522191</v>
+      </c>
+      <c r="K117" t="s">
+        <v>202</v>
+      </c>
+      <c r="L117">
+        <v>21750000</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12">
+      <c r="A118">
+        <v>115</v>
+      </c>
+      <c r="B118">
+        <v>626402</v>
+      </c>
+      <c r="C118" t="s">
+        <v>13</v>
+      </c>
+      <c r="D118" t="s">
+        <v>203</v>
+      </c>
+      <c r="E118" t="s">
+        <v>204</v>
+      </c>
+      <c r="F118" t="s">
+        <v>205</v>
+      </c>
+      <c r="G118" t="s">
+        <v>204</v>
+      </c>
+      <c r="H118">
+        <v>2378</v>
+      </c>
+      <c r="I118" t="s">
+        <v>17</v>
+      </c>
+      <c r="J118">
+        <v>521111</v>
+      </c>
+      <c r="K118" t="s">
+        <v>206</v>
+      </c>
+      <c r="L118">
+        <v>10208000</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12">
+      <c r="A119">
+        <v>116</v>
+      </c>
+      <c r="B119">
+        <v>626402</v>
+      </c>
+      <c r="C119" t="s">
+        <v>13</v>
+      </c>
+      <c r="D119" t="s">
+        <v>207</v>
+      </c>
+      <c r="E119" t="s">
+        <v>208</v>
+      </c>
+      <c r="F119" t="s">
+        <v>209</v>
+      </c>
+      <c r="G119" t="s">
+        <v>208</v>
+      </c>
+      <c r="H119">
+        <v>2378</v>
+      </c>
+      <c r="I119" t="s">
+        <v>17</v>
+      </c>
+      <c r="J119">
+        <v>521111</v>
+      </c>
+      <c r="K119" t="s">
+        <v>210</v>
+      </c>
+      <c r="L119">
+        <v>5104000</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12">
+      <c r="A120">
+        <v>117</v>
+      </c>
+      <c r="B120">
+        <v>626402</v>
+      </c>
+      <c r="C120" t="s">
+        <v>13</v>
+      </c>
+      <c r="D120" t="s">
+        <v>211</v>
+      </c>
+      <c r="E120" t="s">
+        <v>208</v>
+      </c>
+      <c r="F120" t="s">
+        <v>212</v>
+      </c>
+      <c r="G120" t="s">
+        <v>208</v>
+      </c>
+      <c r="H120">
+        <v>2378</v>
+      </c>
+      <c r="I120" t="s">
+        <v>17</v>
+      </c>
+      <c r="J120">
+        <v>511129</v>
+      </c>
+      <c r="K120" t="s">
+        <v>213</v>
+      </c>
+      <c r="L120">
+        <v>24089000</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12">
+      <c r="A121">
+        <v>118</v>
+      </c>
+      <c r="B121">
+        <v>626402</v>
+      </c>
+      <c r="C121" t="s">
+        <v>13</v>
+      </c>
+      <c r="D121" t="s">
+        <v>214</v>
+      </c>
+      <c r="E121" t="s">
+        <v>208</v>
+      </c>
+      <c r="F121" t="s">
+        <v>215</v>
+      </c>
+      <c r="G121" t="s">
+        <v>208</v>
+      </c>
+      <c r="H121">
+        <v>2378</v>
+      </c>
+      <c r="I121" t="s">
+        <v>17</v>
+      </c>
+      <c r="J121">
+        <v>511129</v>
+      </c>
+      <c r="K121" t="s">
+        <v>216</v>
+      </c>
+      <c r="L121">
+        <v>28977000</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12">
+      <c r="A122">
+        <v>119</v>
+      </c>
+      <c r="B122">
+        <v>626402</v>
+      </c>
+      <c r="C122" t="s">
+        <v>13</v>
+      </c>
+      <c r="D122" t="s">
+        <v>217</v>
+      </c>
+      <c r="E122" t="s">
+        <v>208</v>
+      </c>
+      <c r="F122" t="s">
+        <v>218</v>
+      </c>
+      <c r="G122" t="s">
+        <v>208</v>
+      </c>
+      <c r="H122">
+        <v>2378</v>
+      </c>
+      <c r="I122" t="s">
+        <v>17</v>
+      </c>
+      <c r="J122">
+        <v>511129</v>
+      </c>
+      <c r="K122" t="s">
+        <v>219</v>
+      </c>
+      <c r="L122">
+        <v>22005000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>